<commit_message>
Reports of Theoretical and spring '16 experimental analysis
</commit_message>
<xml_diff>
--- a/Theoretical mathematical models.xlsx
+++ b/Theoretical mathematical models.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\husseinz\Desktop\Physics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zainab\Desktop\Physics\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="constant power" sheetId="1" r:id="rId1"/>
     <sheet name="changing power" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -87,9 +87,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -157,15 +157,15 @@
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -184,7 +184,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -237,7 +237,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -496,6 +495,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8394-4C37-B01C-ADA0FBEA090D}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -563,7 +567,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -689,7 +692,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -806,7 +808,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -854,7 +856,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1113,6 +1114,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9B13-460A-93E1-B54A5DBAEF47}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1172,7 +1178,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1290,7 +1295,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1407,7 +1411,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1451,7 +1455,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1710,6 +1713,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A170-410D-B340-EC9DF9D558A9}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1769,7 +1777,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1887,7 +1894,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2004,7 +2010,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2048,7 +2054,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2296,6 +2301,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AD1B-48B0-947B-87EDEE7BBC97}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2355,7 +2365,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2473,7 +2482,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2504,6 +2512,1193 @@
           </c:txPr>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="226911552"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Current</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> and Torque relation given constant Motor speed</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'changing power'!$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Calculated Torque</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'changing power'!$E$4:$E$31</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.7142857142857141E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.11428571428571428</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.17142857142857143</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.22857142857142856</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.2857142857142857</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.34285714285714286</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.45714285714285713</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.51428571428571423</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.5714285714285714</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.62857142857142856</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.68571428571428572</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.74285714285714288</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.8571428571428571</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.91428571428571426</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.97142857142857142</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.0285714285714285</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.0857142857142856</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.1428571428571428</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.2571428571428571</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.3142857142857143</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.3714285714285714</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.4285714285714286</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.4857142857142858</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.5428571428571429</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'changing power'!$C$4:$C$31</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>17.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>22.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>27.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>32.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>37.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>42.5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>47.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>52.5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>57.5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>62.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>67.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FAD5-4BB7-A07B-66910F63D3EF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="226907632"/>
+        <c:axId val="226907072"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="226907632"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Torque (Nm)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="226907072"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="226907072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Current (A)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="226907632"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Current and Motor</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> speed relation given constant Torque</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'changing power'!$G$4:$G$31</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28.571428571428573</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>57.142857142857146</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>85.714285714285708</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>114.28571428571429</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>142.85714285714286</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>171.42857142857142</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>228.57142857142858</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>257.14285714285717</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>285.71428571428572</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>314.28571428571428</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>342.85714285714283</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>371.42857142857144</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>428.57142857142856</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>457.14285714285717</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>485.71428571428572</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>514.28571428571433</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>542.85714285714289</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>571.42857142857144</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>628.57142857142856</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>657.14285714285711</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>685.71428571428567</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>714.28571428571433</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>742.85714285714289</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>771.42857142857144</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'changing power'!$C$4:$C$31</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>17.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>22.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>27.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>32.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>37.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>42.5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>47.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>52.5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>57.5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>62.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>67.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6BE6-425E-871D-CBA400380A3D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="226911552"/>
+        <c:axId val="226910432"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="226911552"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Motor speed (rad/s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="226910432"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="226910432"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Current (A)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2749,6 +3944,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -4298,6 +5573,1038 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4830,7 +7137,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -4860,7 +7173,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -4895,7 +7214,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -4925,7 +7250,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -4935,6 +7266,82 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5019,6 +7426,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -5054,6 +7478,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -5224,30 +7665,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2" t="s">
+      <c r="E2" s="5"/>
+      <c r="F2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="2"/>
+      <c r="G2" s="5"/>
     </row>
     <row r="3" spans="1:7" ht="18.75" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
@@ -5280,20 +7721,20 @@
         <v>80</v>
       </c>
       <c r="C4" s="1">
-        <f t="shared" ref="C4:C31" si="0">A4/B4</f>
+        <f t="shared" ref="C4:C22" si="0">A4/B4</f>
         <v>12.5</v>
       </c>
       <c r="D4" s="1">
         <v>250</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <f t="shared" ref="E4:E31" si="1">A4/D4</f>
         <v>4</v>
       </c>
       <c r="F4" s="1">
         <v>1</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="3">
         <f t="shared" ref="G4:G31" si="2">A4/F4</f>
         <v>1000</v>
       </c>
@@ -5312,14 +7753,14 @@
       <c r="D5" s="1">
         <v>500</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="F5" s="1">
         <v>2</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="3">
         <f t="shared" si="2"/>
         <v>500</v>
       </c>
@@ -5338,14 +7779,14 @@
       <c r="D6" s="1">
         <v>750</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <f t="shared" si="1"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="F6" s="1">
         <v>3</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="3">
         <f t="shared" si="2"/>
         <v>333.33333333333331</v>
       </c>
@@ -5364,14 +7805,14 @@
       <c r="D7" s="1">
         <v>1000</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="F7" s="1">
         <v>4</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="3">
         <f t="shared" si="2"/>
         <v>250</v>
       </c>
@@ -5390,14 +7831,14 @@
       <c r="D8" s="1">
         <v>1250</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
       <c r="F8" s="1">
         <v>5</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="3">
         <f t="shared" si="2"/>
         <v>200</v>
       </c>
@@ -5416,14 +7857,14 @@
       <c r="D9" s="1">
         <v>1500</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="2">
         <f t="shared" si="1"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="F9" s="1">
         <v>6</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="3">
         <f t="shared" si="2"/>
         <v>166.66666666666666</v>
       </c>
@@ -5442,14 +7883,14 @@
       <c r="D10" s="1">
         <v>1750</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="2">
         <f t="shared" si="1"/>
         <v>0.5714285714285714</v>
       </c>
       <c r="F10" s="1">
         <v>7</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="3">
         <f t="shared" si="2"/>
         <v>142.85714285714286</v>
       </c>
@@ -5468,14 +7909,14 @@
       <c r="D11" s="1">
         <v>2000</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="2">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
       <c r="F11" s="1">
         <v>8</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="3">
         <f t="shared" si="2"/>
         <v>125</v>
       </c>
@@ -5494,14 +7935,14 @@
       <c r="D12" s="1">
         <v>2250</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="2">
         <f t="shared" si="1"/>
         <v>0.44444444444444442</v>
       </c>
       <c r="F12" s="1">
         <v>9</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="3">
         <f t="shared" si="2"/>
         <v>111.11111111111111</v>
       </c>
@@ -5520,14 +7961,14 @@
       <c r="D13" s="1">
         <v>2500</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="2">
         <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
       <c r="F13" s="1">
         <v>10</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13" s="3">
         <f t="shared" si="2"/>
         <v>100</v>
       </c>
@@ -5546,14 +7987,14 @@
       <c r="D14" s="1">
         <v>2750</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="2">
         <f t="shared" si="1"/>
         <v>0.36363636363636365</v>
       </c>
       <c r="F14" s="1">
         <v>11</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G14" s="3">
         <f t="shared" si="2"/>
         <v>90.909090909090907</v>
       </c>
@@ -5572,14 +8013,14 @@
       <c r="D15" s="1">
         <v>3000</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="2">
         <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="F15" s="1">
         <v>12</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G15" s="3">
         <f t="shared" si="2"/>
         <v>83.333333333333329</v>
       </c>
@@ -5598,14 +8039,14 @@
       <c r="D16" s="1">
         <v>3250</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="2">
         <f t="shared" si="1"/>
         <v>0.30769230769230771</v>
       </c>
       <c r="F16" s="1">
         <v>13</v>
       </c>
-      <c r="G16" s="4">
+      <c r="G16" s="3">
         <f t="shared" si="2"/>
         <v>76.92307692307692</v>
       </c>
@@ -5624,14 +8065,14 @@
       <c r="D17" s="1">
         <v>3500</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17" s="2">
         <f t="shared" si="1"/>
         <v>0.2857142857142857</v>
       </c>
       <c r="F17" s="1">
         <v>14</v>
       </c>
-      <c r="G17" s="4">
+      <c r="G17" s="3">
         <f t="shared" si="2"/>
         <v>71.428571428571431</v>
       </c>
@@ -5650,14 +8091,14 @@
       <c r="D18" s="1">
         <v>3750</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18" s="2">
         <f t="shared" si="1"/>
         <v>0.26666666666666666</v>
       </c>
       <c r="F18" s="1">
         <v>15</v>
       </c>
-      <c r="G18" s="4">
+      <c r="G18" s="3">
         <f t="shared" si="2"/>
         <v>66.666666666666671</v>
       </c>
@@ -5676,14 +8117,14 @@
       <c r="D19" s="1">
         <v>4000</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E19" s="2">
         <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
       <c r="F19" s="1">
         <v>16</v>
       </c>
-      <c r="G19" s="4">
+      <c r="G19" s="3">
         <f t="shared" si="2"/>
         <v>62.5</v>
       </c>
@@ -5702,14 +8143,14 @@
       <c r="D20" s="1">
         <v>4250</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20" s="2">
         <f t="shared" si="1"/>
         <v>0.23529411764705882</v>
       </c>
       <c r="F20" s="1">
         <v>17</v>
       </c>
-      <c r="G20" s="4">
+      <c r="G20" s="3">
         <f t="shared" si="2"/>
         <v>58.823529411764703</v>
       </c>
@@ -5728,14 +8169,14 @@
       <c r="D21" s="1">
         <v>4500</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E21" s="2">
         <f t="shared" si="1"/>
         <v>0.22222222222222221</v>
       </c>
       <c r="F21" s="1">
         <v>18</v>
       </c>
-      <c r="G21" s="4">
+      <c r="G21" s="3">
         <f t="shared" si="2"/>
         <v>55.555555555555557</v>
       </c>
@@ -5754,14 +8195,14 @@
       <c r="D22" s="1">
         <v>4750</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22" s="2">
         <f t="shared" si="1"/>
         <v>0.21052631578947367</v>
       </c>
       <c r="F22" s="1">
         <v>19</v>
       </c>
-      <c r="G22" s="4">
+      <c r="G22" s="3">
         <f t="shared" si="2"/>
         <v>52.631578947368418</v>
       </c>
@@ -5774,20 +8215,20 @@
         <v>80</v>
       </c>
       <c r="C23" s="1">
-        <f>A23/B24</f>
+        <f t="shared" ref="C23:C30" si="3">A23/B24</f>
         <v>12.5</v>
       </c>
       <c r="D23" s="1">
         <v>5000</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E23" s="2">
         <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="F23" s="1">
         <v>20</v>
       </c>
-      <c r="G23" s="4">
+      <c r="G23" s="3">
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
@@ -5800,20 +8241,20 @@
         <v>80</v>
       </c>
       <c r="C24" s="1">
-        <f>A24/B25</f>
+        <f t="shared" si="3"/>
         <v>12.5</v>
       </c>
       <c r="D24" s="1">
         <v>5250</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E24" s="2">
         <f t="shared" si="1"/>
         <v>0.19047619047619047</v>
       </c>
       <c r="F24" s="1">
         <v>21</v>
       </c>
-      <c r="G24" s="4">
+      <c r="G24" s="3">
         <f t="shared" si="2"/>
         <v>47.61904761904762</v>
       </c>
@@ -5826,20 +8267,20 @@
         <v>80</v>
       </c>
       <c r="C25" s="1">
-        <f>A25/B26</f>
+        <f t="shared" si="3"/>
         <v>12.5</v>
       </c>
       <c r="D25" s="1">
         <v>5500</v>
       </c>
-      <c r="E25" s="3">
+      <c r="E25" s="2">
         <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
       <c r="F25" s="1">
         <v>22</v>
       </c>
-      <c r="G25" s="4">
+      <c r="G25" s="3">
         <f t="shared" si="2"/>
         <v>45.454545454545453</v>
       </c>
@@ -5852,20 +8293,20 @@
         <v>80</v>
       </c>
       <c r="C26" s="1">
-        <f>A26/B27</f>
+        <f t="shared" si="3"/>
         <v>12.5</v>
       </c>
       <c r="D26" s="1">
         <v>5750</v>
       </c>
-      <c r="E26" s="3">
+      <c r="E26" s="2">
         <f t="shared" si="1"/>
         <v>0.17391304347826086</v>
       </c>
       <c r="F26" s="1">
         <v>23</v>
       </c>
-      <c r="G26" s="4">
+      <c r="G26" s="3">
         <f t="shared" si="2"/>
         <v>43.478260869565219</v>
       </c>
@@ -5878,20 +8319,20 @@
         <v>80</v>
       </c>
       <c r="C27" s="1">
-        <f>A27/B28</f>
+        <f t="shared" si="3"/>
         <v>12.5</v>
       </c>
       <c r="D27" s="1">
         <v>6000</v>
       </c>
-      <c r="E27" s="3">
+      <c r="E27" s="2">
         <f t="shared" si="1"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="F27" s="1">
         <v>24</v>
       </c>
-      <c r="G27" s="4">
+      <c r="G27" s="3">
         <f t="shared" si="2"/>
         <v>41.666666666666664</v>
       </c>
@@ -5904,20 +8345,20 @@
         <v>80</v>
       </c>
       <c r="C28" s="1">
-        <f>A28/B29</f>
+        <f t="shared" si="3"/>
         <v>12.5</v>
       </c>
       <c r="D28" s="1">
         <v>6250</v>
       </c>
-      <c r="E28" s="3">
+      <c r="E28" s="2">
         <f t="shared" si="1"/>
         <v>0.16</v>
       </c>
       <c r="F28" s="1">
         <v>25</v>
       </c>
-      <c r="G28" s="4">
+      <c r="G28" s="3">
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
@@ -5930,20 +8371,20 @@
         <v>80</v>
       </c>
       <c r="C29" s="1">
-        <f>A29/B30</f>
+        <f t="shared" si="3"/>
         <v>12.5</v>
       </c>
       <c r="D29" s="1">
         <v>6500</v>
       </c>
-      <c r="E29" s="3">
+      <c r="E29" s="2">
         <f t="shared" si="1"/>
         <v>0.15384615384615385</v>
       </c>
       <c r="F29" s="1">
         <v>26</v>
       </c>
-      <c r="G29" s="4">
+      <c r="G29" s="3">
         <f t="shared" si="2"/>
         <v>38.46153846153846</v>
       </c>
@@ -5956,20 +8397,20 @@
         <v>80</v>
       </c>
       <c r="C30" s="1">
-        <f>A30/B31</f>
+        <f t="shared" si="3"/>
         <v>12.5</v>
       </c>
       <c r="D30" s="1">
         <v>6750</v>
       </c>
-      <c r="E30" s="3">
+      <c r="E30" s="2">
         <f t="shared" si="1"/>
         <v>0.14814814814814814</v>
       </c>
       <c r="F30" s="1">
         <v>27</v>
       </c>
-      <c r="G30" s="4">
+      <c r="G30" s="3">
         <f t="shared" si="2"/>
         <v>37.037037037037038</v>
       </c>
@@ -5988,14 +8429,14 @@
       <c r="D31" s="1">
         <v>7000</v>
       </c>
-      <c r="E31" s="3">
+      <c r="E31" s="2">
         <f t="shared" si="1"/>
         <v>0.14285714285714285</v>
       </c>
       <c r="F31" s="1">
         <v>28</v>
       </c>
-      <c r="G31" s="4">
+      <c r="G31" s="3">
         <f t="shared" si="2"/>
         <v>35.714285714285715</v>
       </c>
@@ -6017,8 +8458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6032,30 +8473,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2" t="s">
+      <c r="E2" s="5"/>
+      <c r="F2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="2"/>
+      <c r="G2" s="5"/>
     </row>
     <row r="3" spans="1:7" ht="18.75" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
@@ -6087,21 +8528,21 @@
       <c r="B4" s="1">
         <v>80</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="4">
         <f>A4/B4</f>
         <v>0</v>
       </c>
       <c r="D4" s="1">
         <v>3500</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <f t="shared" ref="E4:E31" si="0">A4/D4</f>
         <v>0</v>
       </c>
       <c r="F4" s="1">
         <v>7</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="3">
         <f t="shared" ref="G4:G31" si="1">A4/F4</f>
         <v>0</v>
       </c>
@@ -6113,21 +8554,21 @@
       <c r="B5" s="1">
         <v>80</v>
       </c>
-      <c r="C5" s="6">
-        <f t="shared" ref="C4:C22" si="2">A5/B5</f>
+      <c r="C5" s="4">
+        <f t="shared" ref="C5:C22" si="2">A5/B5</f>
         <v>2.5</v>
       </c>
       <c r="D5" s="1">
         <v>3500</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <f t="shared" si="0"/>
         <v>5.7142857142857141E-2</v>
       </c>
       <c r="F5" s="1">
         <v>7</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="3">
         <f t="shared" si="1"/>
         <v>28.571428571428573</v>
       </c>
@@ -6139,21 +8580,21 @@
       <c r="B6" s="1">
         <v>80</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="4">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="D6" s="1">
         <v>3500</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <f t="shared" si="0"/>
         <v>0.11428571428571428</v>
       </c>
       <c r="F6" s="1">
         <v>7</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="3">
         <f t="shared" si="1"/>
         <v>57.142857142857146</v>
       </c>
@@ -6165,21 +8606,21 @@
       <c r="B7" s="1">
         <v>80</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="4">
         <f t="shared" si="2"/>
         <v>7.5</v>
       </c>
       <c r="D7" s="1">
         <v>3500</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <f t="shared" si="0"/>
         <v>0.17142857142857143</v>
       </c>
       <c r="F7" s="1">
         <v>7</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="3">
         <f t="shared" si="1"/>
         <v>85.714285714285708</v>
       </c>
@@ -6191,21 +8632,21 @@
       <c r="B8" s="1">
         <v>80</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="4">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="D8" s="1">
         <v>3500</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <f t="shared" si="0"/>
         <v>0.22857142857142856</v>
       </c>
       <c r="F8" s="1">
         <v>7</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="3">
         <f t="shared" si="1"/>
         <v>114.28571428571429</v>
       </c>
@@ -6217,21 +8658,21 @@
       <c r="B9" s="1">
         <v>80</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="4">
         <f t="shared" si="2"/>
         <v>12.5</v>
       </c>
       <c r="D9" s="1">
         <v>3500</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="2">
         <f t="shared" si="0"/>
         <v>0.2857142857142857</v>
       </c>
       <c r="F9" s="1">
         <v>7</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="3">
         <f t="shared" si="1"/>
         <v>142.85714285714286</v>
       </c>
@@ -6243,21 +8684,21 @@
       <c r="B10" s="1">
         <v>80</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="4">
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="D10" s="1">
         <v>3500</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="2">
         <f t="shared" si="0"/>
         <v>0.34285714285714286</v>
       </c>
       <c r="F10" s="1">
         <v>7</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="3">
         <f t="shared" si="1"/>
         <v>171.42857142857142</v>
       </c>
@@ -6269,21 +8710,21 @@
       <c r="B11" s="1">
         <v>80</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="4">
         <f t="shared" si="2"/>
         <v>17.5</v>
       </c>
       <c r="D11" s="1">
         <v>3500</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="2">
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
       <c r="F11" s="1">
         <v>7</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="3">
         <f t="shared" si="1"/>
         <v>200</v>
       </c>
@@ -6295,21 +8736,21 @@
       <c r="B12" s="1">
         <v>80</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="4">
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="D12" s="1">
         <v>3500</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="2">
         <f t="shared" si="0"/>
         <v>0.45714285714285713</v>
       </c>
       <c r="F12" s="1">
         <v>7</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="3">
         <f t="shared" si="1"/>
         <v>228.57142857142858</v>
       </c>
@@ -6321,21 +8762,21 @@
       <c r="B13" s="1">
         <v>80</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="4">
         <f t="shared" si="2"/>
         <v>22.5</v>
       </c>
       <c r="D13" s="1">
         <v>3500</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="2">
         <f t="shared" si="0"/>
         <v>0.51428571428571423</v>
       </c>
       <c r="F13" s="1">
         <v>7</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13" s="3">
         <f t="shared" si="1"/>
         <v>257.14285714285717</v>
       </c>
@@ -6347,21 +8788,21 @@
       <c r="B14" s="1">
         <v>80</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="4">
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
       <c r="D14" s="1">
         <v>3500</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="2">
         <f t="shared" si="0"/>
         <v>0.5714285714285714</v>
       </c>
       <c r="F14" s="1">
         <v>7</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G14" s="3">
         <f t="shared" si="1"/>
         <v>285.71428571428572</v>
       </c>
@@ -6373,21 +8814,21 @@
       <c r="B15" s="1">
         <v>80</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="4">
         <f t="shared" si="2"/>
         <v>27.5</v>
       </c>
       <c r="D15" s="1">
         <v>3500</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="2">
         <f t="shared" si="0"/>
         <v>0.62857142857142856</v>
       </c>
       <c r="F15" s="1">
         <v>7</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G15" s="3">
         <f t="shared" si="1"/>
         <v>314.28571428571428</v>
       </c>
@@ -6399,21 +8840,21 @@
       <c r="B16" s="1">
         <v>80</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="4">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="D16" s="1">
         <v>3500</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="2">
         <f t="shared" si="0"/>
         <v>0.68571428571428572</v>
       </c>
       <c r="F16" s="1">
         <v>7</v>
       </c>
-      <c r="G16" s="4">
+      <c r="G16" s="3">
         <f t="shared" si="1"/>
         <v>342.85714285714283</v>
       </c>
@@ -6425,21 +8866,21 @@
       <c r="B17" s="1">
         <v>80</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="4">
         <f t="shared" si="2"/>
         <v>32.5</v>
       </c>
       <c r="D17" s="1">
         <v>3500</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17" s="2">
         <f t="shared" si="0"/>
         <v>0.74285714285714288</v>
       </c>
       <c r="F17" s="1">
         <v>7</v>
       </c>
-      <c r="G17" s="4">
+      <c r="G17" s="3">
         <f t="shared" si="1"/>
         <v>371.42857142857144</v>
       </c>
@@ -6451,21 +8892,21 @@
       <c r="B18" s="1">
         <v>80</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C18" s="4">
         <f t="shared" si="2"/>
         <v>35</v>
       </c>
       <c r="D18" s="1">
         <v>3500</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18" s="2">
         <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
       <c r="F18" s="1">
         <v>7</v>
       </c>
-      <c r="G18" s="4">
+      <c r="G18" s="3">
         <f t="shared" si="1"/>
         <v>400</v>
       </c>
@@ -6477,21 +8918,21 @@
       <c r="B19" s="1">
         <v>80</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="4">
         <f t="shared" si="2"/>
         <v>37.5</v>
       </c>
       <c r="D19" s="1">
         <v>3500</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E19" s="2">
         <f t="shared" si="0"/>
         <v>0.8571428571428571</v>
       </c>
       <c r="F19" s="1">
         <v>7</v>
       </c>
-      <c r="G19" s="4">
+      <c r="G19" s="3">
         <f t="shared" si="1"/>
         <v>428.57142857142856</v>
       </c>
@@ -6503,21 +8944,21 @@
       <c r="B20" s="1">
         <v>80</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C20" s="4">
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
       <c r="D20" s="1">
         <v>3500</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20" s="2">
         <f t="shared" si="0"/>
         <v>0.91428571428571426</v>
       </c>
       <c r="F20" s="1">
         <v>7</v>
       </c>
-      <c r="G20" s="4">
+      <c r="G20" s="3">
         <f t="shared" si="1"/>
         <v>457.14285714285717</v>
       </c>
@@ -6529,21 +8970,21 @@
       <c r="B21" s="1">
         <v>80</v>
       </c>
-      <c r="C21" s="6">
+      <c r="C21" s="4">
         <f t="shared" si="2"/>
         <v>42.5</v>
       </c>
       <c r="D21" s="1">
         <v>3500</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E21" s="2">
         <f t="shared" si="0"/>
         <v>0.97142857142857142</v>
       </c>
       <c r="F21" s="1">
         <v>7</v>
       </c>
-      <c r="G21" s="4">
+      <c r="G21" s="3">
         <f t="shared" si="1"/>
         <v>485.71428571428572</v>
       </c>
@@ -6555,21 +8996,21 @@
       <c r="B22" s="1">
         <v>80</v>
       </c>
-      <c r="C22" s="6">
+      <c r="C22" s="4">
         <f t="shared" si="2"/>
         <v>45</v>
       </c>
       <c r="D22" s="1">
         <v>3500</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22" s="2">
         <f t="shared" si="0"/>
         <v>1.0285714285714285</v>
       </c>
       <c r="F22" s="1">
         <v>7</v>
       </c>
-      <c r="G22" s="4">
+      <c r="G22" s="3">
         <f t="shared" si="1"/>
         <v>514.28571428571433</v>
       </c>
@@ -6581,21 +9022,21 @@
       <c r="B23" s="1">
         <v>80</v>
       </c>
-      <c r="C23" s="6">
-        <f>A23/B24</f>
+      <c r="C23" s="4">
+        <f t="shared" ref="C23:C30" si="3">A23/B24</f>
         <v>47.5</v>
       </c>
       <c r="D23" s="1">
         <v>3500</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E23" s="2">
         <f t="shared" si="0"/>
         <v>1.0857142857142856</v>
       </c>
       <c r="F23" s="1">
         <v>7</v>
       </c>
-      <c r="G23" s="4">
+      <c r="G23" s="3">
         <f t="shared" si="1"/>
         <v>542.85714285714289</v>
       </c>
@@ -6607,21 +9048,21 @@
       <c r="B24" s="1">
         <v>80</v>
       </c>
-      <c r="C24" s="6">
-        <f>A24/B25</f>
+      <c r="C24" s="4">
+        <f t="shared" si="3"/>
         <v>50</v>
       </c>
       <c r="D24" s="1">
         <v>3500</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E24" s="2">
         <f t="shared" si="0"/>
         <v>1.1428571428571428</v>
       </c>
       <c r="F24" s="1">
         <v>7</v>
       </c>
-      <c r="G24" s="4">
+      <c r="G24" s="3">
         <f t="shared" si="1"/>
         <v>571.42857142857144</v>
       </c>
@@ -6633,21 +9074,21 @@
       <c r="B25" s="1">
         <v>80</v>
       </c>
-      <c r="C25" s="6">
-        <f>A25/B26</f>
+      <c r="C25" s="4">
+        <f t="shared" si="3"/>
         <v>52.5</v>
       </c>
       <c r="D25" s="1">
         <v>3500</v>
       </c>
-      <c r="E25" s="3">
+      <c r="E25" s="2">
         <f t="shared" si="0"/>
         <v>1.2</v>
       </c>
       <c r="F25" s="1">
         <v>7</v>
       </c>
-      <c r="G25" s="4">
+      <c r="G25" s="3">
         <f t="shared" si="1"/>
         <v>600</v>
       </c>
@@ -6659,21 +9100,21 @@
       <c r="B26" s="1">
         <v>80</v>
       </c>
-      <c r="C26" s="6">
-        <f>A26/B27</f>
+      <c r="C26" s="4">
+        <f t="shared" si="3"/>
         <v>55</v>
       </c>
       <c r="D26" s="1">
         <v>3500</v>
       </c>
-      <c r="E26" s="3">
+      <c r="E26" s="2">
         <f t="shared" si="0"/>
         <v>1.2571428571428571</v>
       </c>
       <c r="F26" s="1">
         <v>7</v>
       </c>
-      <c r="G26" s="4">
+      <c r="G26" s="3">
         <f t="shared" si="1"/>
         <v>628.57142857142856</v>
       </c>
@@ -6685,21 +9126,21 @@
       <c r="B27" s="1">
         <v>80</v>
       </c>
-      <c r="C27" s="6">
-        <f>A27/B28</f>
+      <c r="C27" s="4">
+        <f t="shared" si="3"/>
         <v>57.5</v>
       </c>
       <c r="D27" s="1">
         <v>3500</v>
       </c>
-      <c r="E27" s="3">
+      <c r="E27" s="2">
         <f t="shared" si="0"/>
         <v>1.3142857142857143</v>
       </c>
       <c r="F27" s="1">
         <v>7</v>
       </c>
-      <c r="G27" s="4">
+      <c r="G27" s="3">
         <f t="shared" si="1"/>
         <v>657.14285714285711</v>
       </c>
@@ -6711,21 +9152,21 @@
       <c r="B28" s="1">
         <v>80</v>
       </c>
-      <c r="C28" s="6">
-        <f>A28/B29</f>
+      <c r="C28" s="4">
+        <f t="shared" si="3"/>
         <v>60</v>
       </c>
       <c r="D28" s="1">
         <v>3500</v>
       </c>
-      <c r="E28" s="3">
+      <c r="E28" s="2">
         <f t="shared" si="0"/>
         <v>1.3714285714285714</v>
       </c>
       <c r="F28" s="1">
         <v>7</v>
       </c>
-      <c r="G28" s="4">
+      <c r="G28" s="3">
         <f t="shared" si="1"/>
         <v>685.71428571428567</v>
       </c>
@@ -6737,21 +9178,21 @@
       <c r="B29" s="1">
         <v>80</v>
       </c>
-      <c r="C29" s="6">
-        <f>A29/B30</f>
+      <c r="C29" s="4">
+        <f t="shared" si="3"/>
         <v>62.5</v>
       </c>
       <c r="D29" s="1">
         <v>3500</v>
       </c>
-      <c r="E29" s="3">
+      <c r="E29" s="2">
         <f t="shared" si="0"/>
         <v>1.4285714285714286</v>
       </c>
       <c r="F29" s="1">
         <v>7</v>
       </c>
-      <c r="G29" s="4">
+      <c r="G29" s="3">
         <f t="shared" si="1"/>
         <v>714.28571428571433</v>
       </c>
@@ -6763,21 +9204,21 @@
       <c r="B30" s="1">
         <v>80</v>
       </c>
-      <c r="C30" s="6">
-        <f>A30/B31</f>
+      <c r="C30" s="4">
+        <f t="shared" si="3"/>
         <v>65</v>
       </c>
       <c r="D30" s="1">
         <v>3500</v>
       </c>
-      <c r="E30" s="3">
+      <c r="E30" s="2">
         <f t="shared" si="0"/>
         <v>1.4857142857142858</v>
       </c>
       <c r="F30" s="1">
         <v>7</v>
       </c>
-      <c r="G30" s="4">
+      <c r="G30" s="3">
         <f t="shared" si="1"/>
         <v>742.85714285714289</v>
       </c>
@@ -6789,21 +9230,21 @@
       <c r="B31" s="1">
         <v>80</v>
       </c>
-      <c r="C31" s="6">
+      <c r="C31" s="4">
         <f>A31/B31</f>
         <v>67.5</v>
       </c>
       <c r="D31" s="1">
         <v>3500</v>
       </c>
-      <c r="E31" s="3">
+      <c r="E31" s="2">
         <f t="shared" si="0"/>
         <v>1.5428571428571429</v>
       </c>
       <c r="F31" s="1">
         <v>7</v>
       </c>
-      <c r="G31" s="4">
+      <c r="G31" s="3">
         <f t="shared" si="1"/>
         <v>771.42857142857144</v>
       </c>

</xml_diff>

<commit_message>
Updated Theoretical Mathematical relations
</commit_message>
<xml_diff>
--- a/Theoretical mathematical models.xlsx
+++ b/Theoretical mathematical models.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zainab\Desktop\Physics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\husseinz\Desktop\Physics\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14460" windowHeight="10590" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14460" windowHeight="10590"/>
   </bookViews>
   <sheets>
     <sheet name="constant power" sheetId="1" r:id="rId1"/>
@@ -87,7 +87,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -184,7 +184,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -237,6 +237,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -495,7 +496,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-8394-4C37-B01C-ADA0FBEA090D}"/>
             </c:ext>
@@ -509,11 +510,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="223704832"/>
-        <c:axId val="223701472"/>
+        <c:axId val="419847328"/>
+        <c:axId val="419847888"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="223704832"/>
+        <c:axId val="419847328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -567,6 +568,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -633,12 +635,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="223701472"/>
+        <c:crossAx val="419847888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="223701472"/>
+        <c:axId val="419847888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -692,6 +694,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -758,7 +761,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="223704832"/>
+        <c:crossAx val="419847328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -808,7 +811,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -856,6 +859,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1114,7 +1118,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-9B13-460A-93E1-B54A5DBAEF47}"/>
             </c:ext>
@@ -1128,11 +1132,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="223703712"/>
-        <c:axId val="223700912"/>
+        <c:axId val="419846208"/>
+        <c:axId val="487253200"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="223703712"/>
+        <c:axId val="419846208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1178,6 +1182,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1244,12 +1249,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="223700912"/>
+        <c:crossAx val="487253200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="223700912"/>
+        <c:axId val="487253200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1295,6 +1300,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1361,7 +1367,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="223703712"/>
+        <c:crossAx val="419846208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1411,7 +1417,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1455,6 +1461,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1713,7 +1720,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-A170-410D-B340-EC9DF9D558A9}"/>
             </c:ext>
@@ -1727,11 +1734,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="226907632"/>
-        <c:axId val="226907072"/>
+        <c:axId val="394477344"/>
+        <c:axId val="394477904"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="226907632"/>
+        <c:axId val="394477344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1777,6 +1784,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1843,12 +1851,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="226907072"/>
+        <c:crossAx val="394477904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="226907072"/>
+        <c:axId val="394477904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1894,6 +1902,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1960,7 +1969,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="226907632"/>
+        <c:crossAx val="394477344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2010,7 +2019,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2054,6 +2063,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2301,7 +2311,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-AD1B-48B0-947B-87EDEE7BBC97}"/>
             </c:ext>
@@ -2315,11 +2325,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="226911552"/>
-        <c:axId val="226910432"/>
+        <c:axId val="394480144"/>
+        <c:axId val="394480704"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="226911552"/>
+        <c:axId val="394480144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2365,6 +2375,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2431,12 +2442,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="226910432"/>
+        <c:crossAx val="394480704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="226910432"/>
+        <c:axId val="394480704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2482,6 +2493,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2548,7 +2560,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="226911552"/>
+        <c:crossAx val="394480144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2598,7 +2610,7 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2642,6 +2654,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2900,7 +2913,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-FAD5-4BB7-A07B-66910F63D3EF}"/>
             </c:ext>
@@ -2914,11 +2927,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="226907632"/>
-        <c:axId val="226907072"/>
+        <c:axId val="547088400"/>
+        <c:axId val="547088960"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="226907632"/>
+        <c:axId val="547088400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2964,6 +2977,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3030,12 +3044,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="226907072"/>
+        <c:crossAx val="547088960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="226907072"/>
+        <c:axId val="547088960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3081,6 +3095,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3147,7 +3162,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="226907632"/>
+        <c:crossAx val="547088400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3197,7 +3212,7 @@
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3241,6 +3256,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3488,7 +3504,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-6BE6-425E-871D-CBA400380A3D}"/>
             </c:ext>
@@ -3502,11 +3518,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="226911552"/>
-        <c:axId val="226910432"/>
+        <c:axId val="393693408"/>
+        <c:axId val="393693968"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="226911552"/>
+        <c:axId val="393693408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3552,6 +3568,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3618,12 +3635,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="226910432"/>
+        <c:crossAx val="393693968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="226910432"/>
+        <c:axId val="393693968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3669,6 +3686,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3735,7 +3753,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="226911552"/>
+        <c:crossAx val="393693408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7140,7 +7158,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7176,7 +7194,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7217,7 +7235,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7253,7 +7271,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7289,7 +7307,7 @@
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7327,7 +7345,7 @@
         <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7649,7 +7667,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
@@ -8458,7 +8476,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update to model arrays  a while ago
</commit_message>
<xml_diff>
--- a/Theoretical mathematical models.xlsx
+++ b/Theoretical mathematical models.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\husseinz\Desktop\Physics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zainab\Desktop\Physics\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="constant power" sheetId="1" r:id="rId1"/>
     <sheet name="changing power" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -87,9 +87,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -157,15 +157,15 @@
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -184,7 +184,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -237,7 +237,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -496,6 +495,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8394-4C37-B01C-ADA0FBEA090D}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -563,7 +567,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -689,7 +692,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -806,7 +808,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -854,7 +856,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1113,6 +1114,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9B13-460A-93E1-B54A5DBAEF47}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1172,7 +1178,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1290,7 +1295,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1407,7 +1411,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1451,7 +1455,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1710,6 +1713,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A170-410D-B340-EC9DF9D558A9}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1769,7 +1777,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1887,7 +1894,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2004,7 +2010,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2048,7 +2054,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2296,6 +2301,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AD1B-48B0-947B-87EDEE7BBC97}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2355,7 +2365,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2473,7 +2482,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2504,6 +2512,1193 @@
           </c:txPr>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="226911552"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Current</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> and Torque relation given constant Motor speed</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'changing power'!$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Calculated Torque</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'changing power'!$E$4:$E$31</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.7142857142857141E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.11428571428571428</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.17142857142857143</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.22857142857142856</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.2857142857142857</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.34285714285714286</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.45714285714285713</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.51428571428571423</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.5714285714285714</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.62857142857142856</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.68571428571428572</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.74285714285714288</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.8571428571428571</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.91428571428571426</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.97142857142857142</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.0285714285714285</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.0857142857142856</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.1428571428571428</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.2571428571428571</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.3142857142857143</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.3714285714285714</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.4285714285714286</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.4857142857142858</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.5428571428571429</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'changing power'!$C$4:$C$31</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>17.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>22.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>27.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>32.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>37.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>42.5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>47.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>52.5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>57.5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>62.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>67.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FAD5-4BB7-A07B-66910F63D3EF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="226907632"/>
+        <c:axId val="226907072"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="226907632"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Torque (Nm)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="226907072"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="226907072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Current (A)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="226907632"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Current and Motor</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> speed relation given constant Torque</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'changing power'!$G$4:$G$31</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28.571428571428573</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>57.142857142857146</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>85.714285714285708</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>114.28571428571429</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>142.85714285714286</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>171.42857142857142</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>228.57142857142858</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>257.14285714285717</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>285.71428571428572</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>314.28571428571428</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>342.85714285714283</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>371.42857142857144</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>428.57142857142856</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>457.14285714285717</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>485.71428571428572</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>514.28571428571433</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>542.85714285714289</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>571.42857142857144</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>628.57142857142856</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>657.14285714285711</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>685.71428571428567</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>714.28571428571433</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>742.85714285714289</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>771.42857142857144</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'changing power'!$C$4:$C$31</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>17.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>22.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>27.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>32.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>37.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>42.5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>47.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>52.5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>57.5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>62.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>67.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6BE6-425E-871D-CBA400380A3D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="226911552"/>
+        <c:axId val="226910432"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="226911552"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Motor speed (rad/s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="226910432"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="226910432"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Current (A)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2749,6 +3944,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -4298,6 +5573,1038 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4830,7 +7137,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -4860,7 +7173,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -4895,7 +7214,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -4925,7 +7250,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -4935,6 +7266,82 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5019,6 +7426,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -5054,6 +7478,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -5224,30 +7665,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2" t="s">
+      <c r="E2" s="5"/>
+      <c r="F2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="2"/>
+      <c r="G2" s="5"/>
     </row>
     <row r="3" spans="1:7" ht="18.75" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
@@ -5280,20 +7721,20 @@
         <v>80</v>
       </c>
       <c r="C4" s="1">
-        <f t="shared" ref="C4:C31" si="0">A4/B4</f>
+        <f t="shared" ref="C4:C22" si="0">A4/B4</f>
         <v>12.5</v>
       </c>
       <c r="D4" s="1">
         <v>250</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <f t="shared" ref="E4:E31" si="1">A4/D4</f>
         <v>4</v>
       </c>
       <c r="F4" s="1">
         <v>1</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="3">
         <f t="shared" ref="G4:G31" si="2">A4/F4</f>
         <v>1000</v>
       </c>
@@ -5312,14 +7753,14 @@
       <c r="D5" s="1">
         <v>500</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="F5" s="1">
         <v>2</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="3">
         <f t="shared" si="2"/>
         <v>500</v>
       </c>
@@ -5338,14 +7779,14 @@
       <c r="D6" s="1">
         <v>750</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <f t="shared" si="1"/>
         <v>1.3333333333333333</v>
       </c>
       <c r="F6" s="1">
         <v>3</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="3">
         <f t="shared" si="2"/>
         <v>333.33333333333331</v>
       </c>
@@ -5364,14 +7805,14 @@
       <c r="D7" s="1">
         <v>1000</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="F7" s="1">
         <v>4</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="3">
         <f t="shared" si="2"/>
         <v>250</v>
       </c>
@@ -5390,14 +7831,14 @@
       <c r="D8" s="1">
         <v>1250</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
       <c r="F8" s="1">
         <v>5</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="3">
         <f t="shared" si="2"/>
         <v>200</v>
       </c>
@@ -5416,14 +7857,14 @@
       <c r="D9" s="1">
         <v>1500</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="2">
         <f t="shared" si="1"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="F9" s="1">
         <v>6</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="3">
         <f t="shared" si="2"/>
         <v>166.66666666666666</v>
       </c>
@@ -5442,14 +7883,14 @@
       <c r="D10" s="1">
         <v>1750</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="2">
         <f t="shared" si="1"/>
         <v>0.5714285714285714</v>
       </c>
       <c r="F10" s="1">
         <v>7</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="3">
         <f t="shared" si="2"/>
         <v>142.85714285714286</v>
       </c>
@@ -5468,14 +7909,14 @@
       <c r="D11" s="1">
         <v>2000</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="2">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
       <c r="F11" s="1">
         <v>8</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="3">
         <f t="shared" si="2"/>
         <v>125</v>
       </c>
@@ -5494,14 +7935,14 @@
       <c r="D12" s="1">
         <v>2250</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="2">
         <f t="shared" si="1"/>
         <v>0.44444444444444442</v>
       </c>
       <c r="F12" s="1">
         <v>9</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="3">
         <f t="shared" si="2"/>
         <v>111.11111111111111</v>
       </c>
@@ -5520,14 +7961,14 @@
       <c r="D13" s="1">
         <v>2500</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="2">
         <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
       <c r="F13" s="1">
         <v>10</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13" s="3">
         <f t="shared" si="2"/>
         <v>100</v>
       </c>
@@ -5546,14 +7987,14 @@
       <c r="D14" s="1">
         <v>2750</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="2">
         <f t="shared" si="1"/>
         <v>0.36363636363636365</v>
       </c>
       <c r="F14" s="1">
         <v>11</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G14" s="3">
         <f t="shared" si="2"/>
         <v>90.909090909090907</v>
       </c>
@@ -5572,14 +8013,14 @@
       <c r="D15" s="1">
         <v>3000</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="2">
         <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="F15" s="1">
         <v>12</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G15" s="3">
         <f t="shared" si="2"/>
         <v>83.333333333333329</v>
       </c>
@@ -5598,14 +8039,14 @@
       <c r="D16" s="1">
         <v>3250</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="2">
         <f t="shared" si="1"/>
         <v>0.30769230769230771</v>
       </c>
       <c r="F16" s="1">
         <v>13</v>
       </c>
-      <c r="G16" s="4">
+      <c r="G16" s="3">
         <f t="shared" si="2"/>
         <v>76.92307692307692</v>
       </c>
@@ -5624,14 +8065,14 @@
       <c r="D17" s="1">
         <v>3500</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17" s="2">
         <f t="shared" si="1"/>
         <v>0.2857142857142857</v>
       </c>
       <c r="F17" s="1">
         <v>14</v>
       </c>
-      <c r="G17" s="4">
+      <c r="G17" s="3">
         <f t="shared" si="2"/>
         <v>71.428571428571431</v>
       </c>
@@ -5650,14 +8091,14 @@
       <c r="D18" s="1">
         <v>3750</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18" s="2">
         <f t="shared" si="1"/>
         <v>0.26666666666666666</v>
       </c>
       <c r="F18" s="1">
         <v>15</v>
       </c>
-      <c r="G18" s="4">
+      <c r="G18" s="3">
         <f t="shared" si="2"/>
         <v>66.666666666666671</v>
       </c>
@@ -5676,14 +8117,14 @@
       <c r="D19" s="1">
         <v>4000</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E19" s="2">
         <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
       <c r="F19" s="1">
         <v>16</v>
       </c>
-      <c r="G19" s="4">
+      <c r="G19" s="3">
         <f t="shared" si="2"/>
         <v>62.5</v>
       </c>
@@ -5702,14 +8143,14 @@
       <c r="D20" s="1">
         <v>4250</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20" s="2">
         <f t="shared" si="1"/>
         <v>0.23529411764705882</v>
       </c>
       <c r="F20" s="1">
         <v>17</v>
       </c>
-      <c r="G20" s="4">
+      <c r="G20" s="3">
         <f t="shared" si="2"/>
         <v>58.823529411764703</v>
       </c>
@@ -5728,14 +8169,14 @@
       <c r="D21" s="1">
         <v>4500</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E21" s="2">
         <f t="shared" si="1"/>
         <v>0.22222222222222221</v>
       </c>
       <c r="F21" s="1">
         <v>18</v>
       </c>
-      <c r="G21" s="4">
+      <c r="G21" s="3">
         <f t="shared" si="2"/>
         <v>55.555555555555557</v>
       </c>
@@ -5754,14 +8195,14 @@
       <c r="D22" s="1">
         <v>4750</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22" s="2">
         <f t="shared" si="1"/>
         <v>0.21052631578947367</v>
       </c>
       <c r="F22" s="1">
         <v>19</v>
       </c>
-      <c r="G22" s="4">
+      <c r="G22" s="3">
         <f t="shared" si="2"/>
         <v>52.631578947368418</v>
       </c>
@@ -5774,20 +8215,20 @@
         <v>80</v>
       </c>
       <c r="C23" s="1">
-        <f>A23/B24</f>
+        <f t="shared" ref="C23:C30" si="3">A23/B24</f>
         <v>12.5</v>
       </c>
       <c r="D23" s="1">
         <v>5000</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E23" s="2">
         <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="F23" s="1">
         <v>20</v>
       </c>
-      <c r="G23" s="4">
+      <c r="G23" s="3">
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
@@ -5800,20 +8241,20 @@
         <v>80</v>
       </c>
       <c r="C24" s="1">
-        <f>A24/B25</f>
+        <f t="shared" si="3"/>
         <v>12.5</v>
       </c>
       <c r="D24" s="1">
         <v>5250</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E24" s="2">
         <f t="shared" si="1"/>
         <v>0.19047619047619047</v>
       </c>
       <c r="F24" s="1">
         <v>21</v>
       </c>
-      <c r="G24" s="4">
+      <c r="G24" s="3">
         <f t="shared" si="2"/>
         <v>47.61904761904762</v>
       </c>
@@ -5826,20 +8267,20 @@
         <v>80</v>
       </c>
       <c r="C25" s="1">
-        <f>A25/B26</f>
+        <f t="shared" si="3"/>
         <v>12.5</v>
       </c>
       <c r="D25" s="1">
         <v>5500</v>
       </c>
-      <c r="E25" s="3">
+      <c r="E25" s="2">
         <f t="shared" si="1"/>
         <v>0.18181818181818182</v>
       </c>
       <c r="F25" s="1">
         <v>22</v>
       </c>
-      <c r="G25" s="4">
+      <c r="G25" s="3">
         <f t="shared" si="2"/>
         <v>45.454545454545453</v>
       </c>
@@ -5852,20 +8293,20 @@
         <v>80</v>
       </c>
       <c r="C26" s="1">
-        <f>A26/B27</f>
+        <f t="shared" si="3"/>
         <v>12.5</v>
       </c>
       <c r="D26" s="1">
         <v>5750</v>
       </c>
-      <c r="E26" s="3">
+      <c r="E26" s="2">
         <f t="shared" si="1"/>
         <v>0.17391304347826086</v>
       </c>
       <c r="F26" s="1">
         <v>23</v>
       </c>
-      <c r="G26" s="4">
+      <c r="G26" s="3">
         <f t="shared" si="2"/>
         <v>43.478260869565219</v>
       </c>
@@ -5878,20 +8319,20 @@
         <v>80</v>
       </c>
       <c r="C27" s="1">
-        <f>A27/B28</f>
+        <f t="shared" si="3"/>
         <v>12.5</v>
       </c>
       <c r="D27" s="1">
         <v>6000</v>
       </c>
-      <c r="E27" s="3">
+      <c r="E27" s="2">
         <f t="shared" si="1"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="F27" s="1">
         <v>24</v>
       </c>
-      <c r="G27" s="4">
+      <c r="G27" s="3">
         <f t="shared" si="2"/>
         <v>41.666666666666664</v>
       </c>
@@ -5904,20 +8345,20 @@
         <v>80</v>
       </c>
       <c r="C28" s="1">
-        <f>A28/B29</f>
+        <f t="shared" si="3"/>
         <v>12.5</v>
       </c>
       <c r="D28" s="1">
         <v>6250</v>
       </c>
-      <c r="E28" s="3">
+      <c r="E28" s="2">
         <f t="shared" si="1"/>
         <v>0.16</v>
       </c>
       <c r="F28" s="1">
         <v>25</v>
       </c>
-      <c r="G28" s="4">
+      <c r="G28" s="3">
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
@@ -5930,20 +8371,20 @@
         <v>80</v>
       </c>
       <c r="C29" s="1">
-        <f>A29/B30</f>
+        <f t="shared" si="3"/>
         <v>12.5</v>
       </c>
       <c r="D29" s="1">
         <v>6500</v>
       </c>
-      <c r="E29" s="3">
+      <c r="E29" s="2">
         <f t="shared" si="1"/>
         <v>0.15384615384615385</v>
       </c>
       <c r="F29" s="1">
         <v>26</v>
       </c>
-      <c r="G29" s="4">
+      <c r="G29" s="3">
         <f t="shared" si="2"/>
         <v>38.46153846153846</v>
       </c>
@@ -5956,20 +8397,20 @@
         <v>80</v>
       </c>
       <c r="C30" s="1">
-        <f>A30/B31</f>
+        <f t="shared" si="3"/>
         <v>12.5</v>
       </c>
       <c r="D30" s="1">
         <v>6750</v>
       </c>
-      <c r="E30" s="3">
+      <c r="E30" s="2">
         <f t="shared" si="1"/>
         <v>0.14814814814814814</v>
       </c>
       <c r="F30" s="1">
         <v>27</v>
       </c>
-      <c r="G30" s="4">
+      <c r="G30" s="3">
         <f t="shared" si="2"/>
         <v>37.037037037037038</v>
       </c>
@@ -5988,14 +8429,14 @@
       <c r="D31" s="1">
         <v>7000</v>
       </c>
-      <c r="E31" s="3">
+      <c r="E31" s="2">
         <f t="shared" si="1"/>
         <v>0.14285714285714285</v>
       </c>
       <c r="F31" s="1">
         <v>28</v>
       </c>
-      <c r="G31" s="4">
+      <c r="G31" s="3">
         <f t="shared" si="2"/>
         <v>35.714285714285715</v>
       </c>
@@ -6017,8 +8458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6032,30 +8473,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2" t="s">
+      <c r="E2" s="5"/>
+      <c r="F2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="2"/>
+      <c r="G2" s="5"/>
     </row>
     <row r="3" spans="1:7" ht="18.75" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
@@ -6087,21 +8528,21 @@
       <c r="B4" s="1">
         <v>80</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="4">
         <f>A4/B4</f>
         <v>0</v>
       </c>
       <c r="D4" s="1">
         <v>3500</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <f t="shared" ref="E4:E31" si="0">A4/D4</f>
         <v>0</v>
       </c>
       <c r="F4" s="1">
         <v>7</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="3">
         <f t="shared" ref="G4:G31" si="1">A4/F4</f>
         <v>0</v>
       </c>
@@ -6113,21 +8554,21 @@
       <c r="B5" s="1">
         <v>80</v>
       </c>
-      <c r="C5" s="6">
-        <f t="shared" ref="C4:C22" si="2">A5/B5</f>
+      <c r="C5" s="4">
+        <f t="shared" ref="C5:C22" si="2">A5/B5</f>
         <v>2.5</v>
       </c>
       <c r="D5" s="1">
         <v>3500</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <f t="shared" si="0"/>
         <v>5.7142857142857141E-2</v>
       </c>
       <c r="F5" s="1">
         <v>7</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="3">
         <f t="shared" si="1"/>
         <v>28.571428571428573</v>
       </c>
@@ -6139,21 +8580,21 @@
       <c r="B6" s="1">
         <v>80</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="4">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="D6" s="1">
         <v>3500</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <f t="shared" si="0"/>
         <v>0.11428571428571428</v>
       </c>
       <c r="F6" s="1">
         <v>7</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="3">
         <f t="shared" si="1"/>
         <v>57.142857142857146</v>
       </c>
@@ -6165,21 +8606,21 @@
       <c r="B7" s="1">
         <v>80</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="4">
         <f t="shared" si="2"/>
         <v>7.5</v>
       </c>
       <c r="D7" s="1">
         <v>3500</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <f t="shared" si="0"/>
         <v>0.17142857142857143</v>
       </c>
       <c r="F7" s="1">
         <v>7</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="3">
         <f t="shared" si="1"/>
         <v>85.714285714285708</v>
       </c>
@@ -6191,21 +8632,21 @@
       <c r="B8" s="1">
         <v>80</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="4">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="D8" s="1">
         <v>3500</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <f t="shared" si="0"/>
         <v>0.22857142857142856</v>
       </c>
       <c r="F8" s="1">
         <v>7</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="3">
         <f t="shared" si="1"/>
         <v>114.28571428571429</v>
       </c>
@@ -6217,21 +8658,21 @@
       <c r="B9" s="1">
         <v>80</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="4">
         <f t="shared" si="2"/>
         <v>12.5</v>
       </c>
       <c r="D9" s="1">
         <v>3500</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="2">
         <f t="shared" si="0"/>
         <v>0.2857142857142857</v>
       </c>
       <c r="F9" s="1">
         <v>7</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="3">
         <f t="shared" si="1"/>
         <v>142.85714285714286</v>
       </c>
@@ -6243,21 +8684,21 @@
       <c r="B10" s="1">
         <v>80</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="4">
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="D10" s="1">
         <v>3500</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="2">
         <f t="shared" si="0"/>
         <v>0.34285714285714286</v>
       </c>
       <c r="F10" s="1">
         <v>7</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="3">
         <f t="shared" si="1"/>
         <v>171.42857142857142</v>
       </c>
@@ -6269,21 +8710,21 @@
       <c r="B11" s="1">
         <v>80</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="4">
         <f t="shared" si="2"/>
         <v>17.5</v>
       </c>
       <c r="D11" s="1">
         <v>3500</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="2">
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
       <c r="F11" s="1">
         <v>7</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="3">
         <f t="shared" si="1"/>
         <v>200</v>
       </c>
@@ -6295,21 +8736,21 @@
       <c r="B12" s="1">
         <v>80</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="4">
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="D12" s="1">
         <v>3500</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="2">
         <f t="shared" si="0"/>
         <v>0.45714285714285713</v>
       </c>
       <c r="F12" s="1">
         <v>7</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="3">
         <f t="shared" si="1"/>
         <v>228.57142857142858</v>
       </c>
@@ -6321,21 +8762,21 @@
       <c r="B13" s="1">
         <v>80</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="4">
         <f t="shared" si="2"/>
         <v>22.5</v>
       </c>
       <c r="D13" s="1">
         <v>3500</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="2">
         <f t="shared" si="0"/>
         <v>0.51428571428571423</v>
       </c>
       <c r="F13" s="1">
         <v>7</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13" s="3">
         <f t="shared" si="1"/>
         <v>257.14285714285717</v>
       </c>
@@ -6347,21 +8788,21 @@
       <c r="B14" s="1">
         <v>80</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="4">
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
       <c r="D14" s="1">
         <v>3500</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="2">
         <f t="shared" si="0"/>
         <v>0.5714285714285714</v>
       </c>
       <c r="F14" s="1">
         <v>7</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G14" s="3">
         <f t="shared" si="1"/>
         <v>285.71428571428572</v>
       </c>
@@ -6373,21 +8814,21 @@
       <c r="B15" s="1">
         <v>80</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="4">
         <f t="shared" si="2"/>
         <v>27.5</v>
       </c>
       <c r="D15" s="1">
         <v>3500</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="2">
         <f t="shared" si="0"/>
         <v>0.62857142857142856</v>
       </c>
       <c r="F15" s="1">
         <v>7</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G15" s="3">
         <f t="shared" si="1"/>
         <v>314.28571428571428</v>
       </c>
@@ -6399,21 +8840,21 @@
       <c r="B16" s="1">
         <v>80</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="4">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="D16" s="1">
         <v>3500</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="2">
         <f t="shared" si="0"/>
         <v>0.68571428571428572</v>
       </c>
       <c r="F16" s="1">
         <v>7</v>
       </c>
-      <c r="G16" s="4">
+      <c r="G16" s="3">
         <f t="shared" si="1"/>
         <v>342.85714285714283</v>
       </c>
@@ -6425,21 +8866,21 @@
       <c r="B17" s="1">
         <v>80</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="4">
         <f t="shared" si="2"/>
         <v>32.5</v>
       </c>
       <c r="D17" s="1">
         <v>3500</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17" s="2">
         <f t="shared" si="0"/>
         <v>0.74285714285714288</v>
       </c>
       <c r="F17" s="1">
         <v>7</v>
       </c>
-      <c r="G17" s="4">
+      <c r="G17" s="3">
         <f t="shared" si="1"/>
         <v>371.42857142857144</v>
       </c>
@@ -6451,21 +8892,21 @@
       <c r="B18" s="1">
         <v>80</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C18" s="4">
         <f t="shared" si="2"/>
         <v>35</v>
       </c>
       <c r="D18" s="1">
         <v>3500</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18" s="2">
         <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
       <c r="F18" s="1">
         <v>7</v>
       </c>
-      <c r="G18" s="4">
+      <c r="G18" s="3">
         <f t="shared" si="1"/>
         <v>400</v>
       </c>
@@ -6477,21 +8918,21 @@
       <c r="B19" s="1">
         <v>80</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="4">
         <f t="shared" si="2"/>
         <v>37.5</v>
       </c>
       <c r="D19" s="1">
         <v>3500</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E19" s="2">
         <f t="shared" si="0"/>
         <v>0.8571428571428571</v>
       </c>
       <c r="F19" s="1">
         <v>7</v>
       </c>
-      <c r="G19" s="4">
+      <c r="G19" s="3">
         <f t="shared" si="1"/>
         <v>428.57142857142856</v>
       </c>
@@ -6503,21 +8944,21 @@
       <c r="B20" s="1">
         <v>80</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C20" s="4">
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
       <c r="D20" s="1">
         <v>3500</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20" s="2">
         <f t="shared" si="0"/>
         <v>0.91428571428571426</v>
       </c>
       <c r="F20" s="1">
         <v>7</v>
       </c>
-      <c r="G20" s="4">
+      <c r="G20" s="3">
         <f t="shared" si="1"/>
         <v>457.14285714285717</v>
       </c>
@@ -6529,21 +8970,21 @@
       <c r="B21" s="1">
         <v>80</v>
       </c>
-      <c r="C21" s="6">
+      <c r="C21" s="4">
         <f t="shared" si="2"/>
         <v>42.5</v>
       </c>
       <c r="D21" s="1">
         <v>3500</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E21" s="2">
         <f t="shared" si="0"/>
         <v>0.97142857142857142</v>
       </c>
       <c r="F21" s="1">
         <v>7</v>
       </c>
-      <c r="G21" s="4">
+      <c r="G21" s="3">
         <f t="shared" si="1"/>
         <v>485.71428571428572</v>
       </c>
@@ -6555,21 +8996,21 @@
       <c r="B22" s="1">
         <v>80</v>
       </c>
-      <c r="C22" s="6">
+      <c r="C22" s="4">
         <f t="shared" si="2"/>
         <v>45</v>
       </c>
       <c r="D22" s="1">
         <v>3500</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22" s="2">
         <f t="shared" si="0"/>
         <v>1.0285714285714285</v>
       </c>
       <c r="F22" s="1">
         <v>7</v>
       </c>
-      <c r="G22" s="4">
+      <c r="G22" s="3">
         <f t="shared" si="1"/>
         <v>514.28571428571433</v>
       </c>
@@ -6581,21 +9022,21 @@
       <c r="B23" s="1">
         <v>80</v>
       </c>
-      <c r="C23" s="6">
-        <f>A23/B24</f>
+      <c r="C23" s="4">
+        <f t="shared" ref="C23:C30" si="3">A23/B24</f>
         <v>47.5</v>
       </c>
       <c r="D23" s="1">
         <v>3500</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E23" s="2">
         <f t="shared" si="0"/>
         <v>1.0857142857142856</v>
       </c>
       <c r="F23" s="1">
         <v>7</v>
       </c>
-      <c r="G23" s="4">
+      <c r="G23" s="3">
         <f t="shared" si="1"/>
         <v>542.85714285714289</v>
       </c>
@@ -6607,21 +9048,21 @@
       <c r="B24" s="1">
         <v>80</v>
       </c>
-      <c r="C24" s="6">
-        <f>A24/B25</f>
+      <c r="C24" s="4">
+        <f t="shared" si="3"/>
         <v>50</v>
       </c>
       <c r="D24" s="1">
         <v>3500</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E24" s="2">
         <f t="shared" si="0"/>
         <v>1.1428571428571428</v>
       </c>
       <c r="F24" s="1">
         <v>7</v>
       </c>
-      <c r="G24" s="4">
+      <c r="G24" s="3">
         <f t="shared" si="1"/>
         <v>571.42857142857144</v>
       </c>
@@ -6633,21 +9074,21 @@
       <c r="B25" s="1">
         <v>80</v>
       </c>
-      <c r="C25" s="6">
-        <f>A25/B26</f>
+      <c r="C25" s="4">
+        <f t="shared" si="3"/>
         <v>52.5</v>
       </c>
       <c r="D25" s="1">
         <v>3500</v>
       </c>
-      <c r="E25" s="3">
+      <c r="E25" s="2">
         <f t="shared" si="0"/>
         <v>1.2</v>
       </c>
       <c r="F25" s="1">
         <v>7</v>
       </c>
-      <c r="G25" s="4">
+      <c r="G25" s="3">
         <f t="shared" si="1"/>
         <v>600</v>
       </c>
@@ -6659,21 +9100,21 @@
       <c r="B26" s="1">
         <v>80</v>
       </c>
-      <c r="C26" s="6">
-        <f>A26/B27</f>
+      <c r="C26" s="4">
+        <f t="shared" si="3"/>
         <v>55</v>
       </c>
       <c r="D26" s="1">
         <v>3500</v>
       </c>
-      <c r="E26" s="3">
+      <c r="E26" s="2">
         <f t="shared" si="0"/>
         <v>1.2571428571428571</v>
       </c>
       <c r="F26" s="1">
         <v>7</v>
       </c>
-      <c r="G26" s="4">
+      <c r="G26" s="3">
         <f t="shared" si="1"/>
         <v>628.57142857142856</v>
       </c>
@@ -6685,21 +9126,21 @@
       <c r="B27" s="1">
         <v>80</v>
       </c>
-      <c r="C27" s="6">
-        <f>A27/B28</f>
+      <c r="C27" s="4">
+        <f t="shared" si="3"/>
         <v>57.5</v>
       </c>
       <c r="D27" s="1">
         <v>3500</v>
       </c>
-      <c r="E27" s="3">
+      <c r="E27" s="2">
         <f t="shared" si="0"/>
         <v>1.3142857142857143</v>
       </c>
       <c r="F27" s="1">
         <v>7</v>
       </c>
-      <c r="G27" s="4">
+      <c r="G27" s="3">
         <f t="shared" si="1"/>
         <v>657.14285714285711</v>
       </c>
@@ -6711,21 +9152,21 @@
       <c r="B28" s="1">
         <v>80</v>
       </c>
-      <c r="C28" s="6">
-        <f>A28/B29</f>
+      <c r="C28" s="4">
+        <f t="shared" si="3"/>
         <v>60</v>
       </c>
       <c r="D28" s="1">
         <v>3500</v>
       </c>
-      <c r="E28" s="3">
+      <c r="E28" s="2">
         <f t="shared" si="0"/>
         <v>1.3714285714285714</v>
       </c>
       <c r="F28" s="1">
         <v>7</v>
       </c>
-      <c r="G28" s="4">
+      <c r="G28" s="3">
         <f t="shared" si="1"/>
         <v>685.71428571428567</v>
       </c>
@@ -6737,21 +9178,21 @@
       <c r="B29" s="1">
         <v>80</v>
       </c>
-      <c r="C29" s="6">
-        <f>A29/B30</f>
+      <c r="C29" s="4">
+        <f t="shared" si="3"/>
         <v>62.5</v>
       </c>
       <c r="D29" s="1">
         <v>3500</v>
       </c>
-      <c r="E29" s="3">
+      <c r="E29" s="2">
         <f t="shared" si="0"/>
         <v>1.4285714285714286</v>
       </c>
       <c r="F29" s="1">
         <v>7</v>
       </c>
-      <c r="G29" s="4">
+      <c r="G29" s="3">
         <f t="shared" si="1"/>
         <v>714.28571428571433</v>
       </c>
@@ -6763,21 +9204,21 @@
       <c r="B30" s="1">
         <v>80</v>
       </c>
-      <c r="C30" s="6">
-        <f>A30/B31</f>
+      <c r="C30" s="4">
+        <f t="shared" si="3"/>
         <v>65</v>
       </c>
       <c r="D30" s="1">
         <v>3500</v>
       </c>
-      <c r="E30" s="3">
+      <c r="E30" s="2">
         <f t="shared" si="0"/>
         <v>1.4857142857142858</v>
       </c>
       <c r="F30" s="1">
         <v>7</v>
       </c>
-      <c r="G30" s="4">
+      <c r="G30" s="3">
         <f t="shared" si="1"/>
         <v>742.85714285714289</v>
       </c>
@@ -6789,21 +9230,21 @@
       <c r="B31" s="1">
         <v>80</v>
       </c>
-      <c r="C31" s="6">
+      <c r="C31" s="4">
         <f>A31/B31</f>
         <v>67.5</v>
       </c>
       <c r="D31" s="1">
         <v>3500</v>
       </c>
-      <c r="E31" s="3">
+      <c r="E31" s="2">
         <f t="shared" si="0"/>
         <v>1.5428571428571429</v>
       </c>
       <c r="F31" s="1">
         <v>7</v>
       </c>
-      <c r="G31" s="4">
+      <c r="G31" s="3">
         <f t="shared" si="1"/>
         <v>771.42857142857144</v>
       </c>

</xml_diff>